<commit_message>
Alias [Instytut Archeologii i Etnologii Polskiej Akademii Nauk. Oddział Kraków]
</commit_message>
<xml_diff>
--- a/bg-umw/aliasy_wydawcow.xlsx
+++ b/bg-umw/aliasy_wydawcow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpasternak/Programowanie/bpp-assets/bg-umw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22BC9DA1-71F7-7640-AC7C-1EFE98F6BB7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AD4985-E97F-6A41-B3DD-4B7CC517030C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="6760" windowWidth="36100" windowHeight="22060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="460" windowWidth="36100" windowHeight="22040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t>Wydawnictwo</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>ALIAS</t>
+  </si>
+  <si>
+    <t>[Instytut Archeologii i Etnologii Polskiej Akademii Nauk. Oddział Kraków]</t>
+  </si>
+  <si>
+    <t>Instytut Archeologii i Etnologii Polskiej Akademii Nauk</t>
   </si>
 </sst>
 </file>
@@ -361,10 +367,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB6B48E0-5FF0-9741-A864-D657105640BB}" name="Tabela1" displayName="Tabela1" ref="A1:B50" totalsRowShown="0">
-  <autoFilter ref="A1:B50" xr:uid="{AA07A4D0-4776-DC40-BD3B-05C1CC52143B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B50">
-    <sortCondition ref="A1:A50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB6B48E0-5FF0-9741-A864-D657105640BB}" name="Tabela1" displayName="Tabela1" ref="A1:B51" totalsRowShown="0">
+  <autoFilter ref="A1:B51" xr:uid="{AA07A4D0-4776-DC40-BD3B-05C1CC52143B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B51">
+    <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0EA3FC83-906A-9F43-BDC7-457896DA0936}" name="ALIAS"/>
@@ -640,7 +646,7 @@
   <dimension ref="A1:C727"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1083,24 +1089,30 @@
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>39</v>
+      <c r="A49" t="s">
+        <v>85</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>